<commit_message>
All finished with categories
</commit_message>
<xml_diff>
--- a/phones.xlsx
+++ b/phones.xlsx
@@ -12,10 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="78">
-  <si>
-    <t>Категория</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="74">
   <si>
     <t>Модель</t>
   </si>
@@ -51,9 +48,6 @@
   </si>
   <si>
     <t>48 mm</t>
-  </si>
-  <si>
-    <t>Смартфон</t>
   </si>
   <si>
     <t>iPhone 13 Pro max</t>
@@ -205,9 +199,6 @@
     <t>Samsung Galaxy S24 Ultra</t>
   </si>
   <si>
-    <t>Apple Watch</t>
-  </si>
-  <si>
     <t>Apple Watch 8</t>
   </si>
   <si>
@@ -230,9 +221,6 @@
   </si>
   <si>
     <t>16/512</t>
-  </si>
-  <si>
-    <t>Mac</t>
   </si>
   <si>
     <t>MacBook Pro 16 M1 Pro</t>
@@ -313,12 +301,9 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
@@ -327,19 +312,10 @@
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="17" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
@@ -563,8 +539,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="19.5"/>
-    <col customWidth="1" min="3" max="27" width="11.13"/>
+    <col customWidth="1" min="1" max="1" width="19.5"/>
+    <col customWidth="1" min="2" max="26" width="11.13"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -574,981 +550,829 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+    </row>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
-    </row>
-    <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="5" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="2">
+        <v>45000.0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>48000.0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>55000.0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>65000.0</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="2">
+        <v>40000.0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>43000.0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>47000.0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>51000.0</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="3">
+      <c r="B4" s="4"/>
+      <c r="C4" s="2">
+        <v>30000.0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>34000.0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>37000.0</v>
+      </c>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="2">
+        <v>27000.0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>31000.0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>35000.0</v>
+      </c>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="2">
+        <v>30000.0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>34000.0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>40000.0</v>
+      </c>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="2">
+        <v>27000.0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>30000.0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>34000.0</v>
+      </c>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2">
+        <v>20000.0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>22000.0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>24000.0</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="2">
+        <v>18000.0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>20000.0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>24000.0</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2">
+        <v>21000.0</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="2">
+        <v>24000.0</v>
+      </c>
+      <c r="E10" s="2">
+        <v>27000.0</v>
+      </c>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="2">
+        <v>18000.0</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="2">
+        <v>21000.0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>24000.0</v>
+      </c>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="2">
+        <v>12000.0</v>
+      </c>
+      <c r="C12" s="2">
+        <v>13000.0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>15000.0</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="2">
+        <v>12000.0</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="2">
+        <v>15000.0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>16000.0</v>
+      </c>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2">
+        <v>11000.0</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="2">
+        <v>12000.0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>13000.0</v>
+      </c>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="A15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="2">
+        <v>10000.0</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="2">
+        <v>12000.0</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="2">
+        <v>10000.0</v>
+      </c>
+      <c r="C16" s="2">
+        <v>11000.0</v>
+      </c>
+      <c r="D16" s="2">
+        <v>12000.0</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="A18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="2">
+        <v>10000.0</v>
+      </c>
+      <c r="C19" s="2">
+        <v>12000.0</v>
+      </c>
+      <c r="D19" s="2">
+        <v>13000.0</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" ht="15.75" customHeight="1">
+      <c r="A20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="2">
+        <v>40000.0</v>
+      </c>
+      <c r="D20" s="2">
+        <v>43000.0</v>
+      </c>
+      <c r="E20" s="2">
         <v>45000.0</v>
       </c>
-      <c r="E2" s="3">
-        <v>48000.0</v>
-      </c>
-      <c r="F2" s="3">
-        <v>55000.0</v>
-      </c>
-      <c r="G2" s="3">
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="2">
+        <v>46000.0</v>
+      </c>
+      <c r="D21" s="2">
+        <v>49000.0</v>
+      </c>
+      <c r="E21" s="2">
+        <v>52000.0</v>
+      </c>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="2">
+        <v>52000.0</v>
+      </c>
+      <c r="D22" s="2">
+        <v>57000.0</v>
+      </c>
+      <c r="E22" s="2">
+        <v>62000.0</v>
+      </c>
+      <c r="F22" s="2">
         <v>65000.0</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="3">
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="2">
+        <v>61000.0</v>
+      </c>
+      <c r="D23" s="2">
+        <v>67000.0</v>
+      </c>
+      <c r="E23" s="2">
+        <v>71000.0</v>
+      </c>
+      <c r="F23" s="2">
+        <v>79000.0</v>
+      </c>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="2">
+        <v>52000.0</v>
+      </c>
+      <c r="D24" s="2">
+        <v>58000.0</v>
+      </c>
+      <c r="E24" s="2">
+        <v>65000.0</v>
+      </c>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="2">
+        <v>70000.0</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="2">
+        <v>74000.0</v>
+      </c>
+      <c r="E26" s="2">
+        <v>82000.0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>85000.0</v>
+      </c>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="2">
+        <v>83000.0</v>
+      </c>
+      <c r="E27" s="2">
+        <v>88000.0</v>
+      </c>
+      <c r="F27" s="2">
+        <v>94000.0</v>
+      </c>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4">
+        <v>12000.0</v>
+      </c>
+      <c r="D28" s="2">
+        <v>18000.0</v>
+      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4">
+        <v>11000.0</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="3"/>
+    </row>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4">
+        <v>18000.0</v>
+      </c>
+      <c r="D30" s="2">
+        <v>21000.0</v>
+      </c>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4">
+        <v>27000.0</v>
+      </c>
+      <c r="D31" s="2">
+        <v>32000.0</v>
+      </c>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4">
+        <v>32000.0</v>
+      </c>
+      <c r="D32" s="2">
+        <v>38000.0</v>
+      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4">
+        <v>45000.0</v>
+      </c>
+      <c r="D33" s="2">
+        <v>50000.0</v>
+      </c>
+      <c r="E33" s="2">
+        <v>60000.0</v>
+      </c>
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4">
+        <v>25000.0</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="A35" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4">
+        <v>20000.0</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="A36" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4">
+        <v>12000.0</v>
+      </c>
+      <c r="D36" s="2">
+        <v>20000.0</v>
+      </c>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" ht="15.75" customHeight="1">
+      <c r="A37" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4">
+        <v>18000.0</v>
+      </c>
+      <c r="D37" s="2">
+        <v>24000.0</v>
+      </c>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="A38" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4">
+        <v>34000.0</v>
+      </c>
+      <c r="D38" s="2">
         <v>40000.0</v>
       </c>
-      <c r="E3" s="3">
-        <v>43000.0</v>
-      </c>
-      <c r="F3" s="3">
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+    </row>
+    <row r="39" ht="15.75" customHeight="1">
+      <c r="A39" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4">
+        <v>30000.0</v>
+      </c>
+      <c r="D39" s="2">
+        <v>33000.0</v>
+      </c>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" ht="15.75" customHeight="1">
+      <c r="A40" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="2">
+        <v>40000.0</v>
+      </c>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" ht="15.75" customHeight="1">
+      <c r="A41" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="2">
+        <v>45000.0</v>
+      </c>
+      <c r="E41" s="2">
         <v>47000.0</v>
       </c>
-      <c r="G3" s="3">
-        <v>51000.0</v>
-      </c>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="3">
-        <v>30000.0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>34000.0</v>
-      </c>
-      <c r="F4" s="3">
+      <c r="F41" s="2"/>
+    </row>
+    <row r="42" ht="15.75" customHeight="1">
+      <c r="A42" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4">
+        <v>38000.0</v>
+      </c>
+      <c r="D42" s="2">
+        <v>42000.0</v>
+      </c>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" ht="15.75" customHeight="1">
+      <c r="A43" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="2">
+        <v>50000.0</v>
+      </c>
+      <c r="E43" s="2">
+        <v>60000.0</v>
+      </c>
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" ht="15.75" customHeight="1">
+      <c r="A44" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="2">
+        <v>60000.0</v>
+      </c>
+      <c r="E44" s="2">
+        <v>70000.0</v>
+      </c>
+      <c r="F44" s="2"/>
+    </row>
+    <row r="45" ht="15.75" customHeight="1">
+      <c r="A45" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="H45" s="5">
+        <v>13000.0</v>
+      </c>
+      <c r="K45" s="5">
+        <v>15000.0</v>
+      </c>
+    </row>
+    <row r="46" ht="15.75" customHeight="1">
+      <c r="A46" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="H46" s="5">
+        <v>17000.0</v>
+      </c>
+      <c r="K46" s="5">
+        <v>19000.0</v>
+      </c>
+    </row>
+    <row r="47" ht="15.75" customHeight="1">
+      <c r="A47" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="5">
         <v>37000.0</v>
       </c>
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="3">
-        <v>27000.0</v>
-      </c>
-      <c r="E5" s="3">
-        <v>31000.0</v>
-      </c>
-      <c r="F5" s="3">
-        <v>35000.0</v>
-      </c>
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="3">
-        <v>30000.0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>34000.0</v>
-      </c>
-      <c r="F6" s="3">
-        <v>40000.0</v>
-      </c>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="3">
-        <v>27000.0</v>
-      </c>
-      <c r="E7" s="3">
-        <v>30000.0</v>
-      </c>
-      <c r="F7" s="3">
-        <v>34000.0</v>
-      </c>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="3">
-        <v>20000.0</v>
-      </c>
-      <c r="D8" s="3">
-        <v>22000.0</v>
-      </c>
-      <c r="E8" s="3">
-        <v>24000.0</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="3">
-        <v>18000.0</v>
-      </c>
-      <c r="D9" s="3">
-        <v>20000.0</v>
-      </c>
-      <c r="E9" s="3">
-        <v>24000.0</v>
-      </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="3">
-        <v>21000.0</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="3">
-        <v>24000.0</v>
-      </c>
-      <c r="F10" s="3">
-        <v>27000.0</v>
-      </c>
-      <c r="G10" s="6"/>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="3">
-        <v>18000.0</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="3">
-        <v>21000.0</v>
-      </c>
-      <c r="F11" s="3">
-        <v>24000.0</v>
-      </c>
-      <c r="G11" s="6"/>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="3">
-        <v>12000.0</v>
-      </c>
-      <c r="D12" s="3">
-        <v>13000.0</v>
-      </c>
-      <c r="E12" s="3">
-        <v>15000.0</v>
-      </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-    </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="3">
-        <v>12000.0</v>
-      </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="3">
-        <v>15000.0</v>
-      </c>
-      <c r="F13" s="3">
-        <v>16000.0</v>
-      </c>
-      <c r="G13" s="6"/>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="3">
-        <v>11000.0</v>
-      </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="3">
-        <v>12000.0</v>
-      </c>
-      <c r="F14" s="3">
-        <v>13000.0</v>
-      </c>
-      <c r="G14" s="6"/>
-    </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="3">
+    </row>
+    <row r="48" ht="15.75" customHeight="1">
+      <c r="A48" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="5">
+        <v>8000.0</v>
+      </c>
+      <c r="J48" s="5">
         <v>10000.0</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="3">
-        <v>12000.0</v>
-      </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-    </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="3">
-        <v>10000.0</v>
-      </c>
-      <c r="D16" s="3">
-        <v>11000.0</v>
-      </c>
-      <c r="E16" s="3">
-        <v>12000.0</v>
-      </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-    </row>
-    <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-    </row>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-    </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="3">
-        <v>10000.0</v>
-      </c>
-      <c r="D19" s="3">
-        <v>12000.0</v>
-      </c>
-      <c r="E19" s="3">
-        <v>13000.0</v>
-      </c>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-    </row>
-    <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="3">
-        <v>40000.0</v>
-      </c>
-      <c r="E20" s="3">
-        <v>43000.0</v>
-      </c>
-      <c r="F20" s="3">
-        <v>45000.0</v>
-      </c>
-      <c r="G20" s="6"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="3">
-        <v>46000.0</v>
-      </c>
-      <c r="E21" s="3">
-        <v>49000.0</v>
-      </c>
-      <c r="F21" s="3">
-        <v>52000.0</v>
-      </c>
-      <c r="G21" s="6"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="3">
-        <v>52000.0</v>
-      </c>
-      <c r="E22" s="3">
-        <v>57000.0</v>
-      </c>
-      <c r="F22" s="3">
-        <v>62000.0</v>
-      </c>
-      <c r="G22" s="3">
-        <v>65000.0</v>
-      </c>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="3">
-        <v>61000.0</v>
-      </c>
-      <c r="E23" s="3">
-        <v>67000.0</v>
-      </c>
-      <c r="F23" s="3">
-        <v>71000.0</v>
-      </c>
-      <c r="G23" s="3">
-        <v>79000.0</v>
-      </c>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="3">
-        <v>52000.0</v>
-      </c>
-      <c r="E24" s="3">
-        <v>58000.0</v>
-      </c>
-      <c r="F24" s="3">
-        <v>65000.0</v>
-      </c>
-      <c r="G24" s="6"/>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="3">
-        <v>70000.0</v>
-      </c>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E26" s="3">
-        <v>74000.0</v>
-      </c>
-      <c r="F26" s="3">
-        <v>82000.0</v>
-      </c>
-      <c r="G26" s="3">
-        <v>85000.0</v>
-      </c>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="3">
-        <v>83000.0</v>
-      </c>
-      <c r="F27" s="3">
-        <v>88000.0</v>
-      </c>
-      <c r="G27" s="3">
-        <v>94000.0</v>
-      </c>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6">
-        <v>12000.0</v>
-      </c>
-      <c r="E28" s="3">
-        <v>18000.0</v>
-      </c>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6">
-        <v>11000.0</v>
-      </c>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="4"/>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6">
-        <v>18000.0</v>
-      </c>
-      <c r="E30" s="3">
-        <v>21000.0</v>
-      </c>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6">
-        <v>27000.0</v>
-      </c>
-      <c r="E31" s="3">
-        <v>32000.0</v>
-      </c>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6">
-        <v>32000.0</v>
-      </c>
-      <c r="E32" s="3">
-        <v>38000.0</v>
-      </c>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6">
-        <v>45000.0</v>
-      </c>
-      <c r="E33" s="3">
-        <v>50000.0</v>
-      </c>
-      <c r="F33" s="3">
-        <v>60000.0</v>
-      </c>
-      <c r="G33" s="3"/>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6">
-        <v>25000.0</v>
-      </c>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6">
-        <v>20000.0</v>
-      </c>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-    </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6">
-        <v>12000.0</v>
-      </c>
-      <c r="E36" s="3">
-        <v>20000.0</v>
-      </c>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-    </row>
-    <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6">
-        <v>18000.0</v>
-      </c>
-      <c r="E37" s="3">
-        <v>24000.0</v>
-      </c>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-    </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6">
-        <v>34000.0</v>
-      </c>
-      <c r="E38" s="3">
-        <v>40000.0</v>
-      </c>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-    </row>
-    <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6">
-        <v>30000.0</v>
-      </c>
-      <c r="E39" s="3">
-        <v>33000.0</v>
-      </c>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-    </row>
-    <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="3">
-        <v>40000.0</v>
-      </c>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-    </row>
-    <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="3">
-        <v>45000.0</v>
-      </c>
-      <c r="F41" s="3">
-        <v>47000.0</v>
-      </c>
-      <c r="G41" s="3"/>
-    </row>
-    <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6">
-        <v>38000.0</v>
-      </c>
-      <c r="E42" s="3">
-        <v>42000.0</v>
-      </c>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-    </row>
-    <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="3">
-        <v>50000.0</v>
-      </c>
-      <c r="F43" s="3">
-        <v>60000.0</v>
-      </c>
-      <c r="G43" s="3"/>
-    </row>
-    <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="3">
-        <v>60000.0</v>
-      </c>
-      <c r="F44" s="3">
-        <v>70000.0</v>
-      </c>
-      <c r="G44" s="3"/>
-    </row>
-    <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="I45" s="7">
-        <v>13000.0</v>
-      </c>
-      <c r="L45" s="7">
-        <v>15000.0</v>
-      </c>
-    </row>
-    <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="I46" s="7">
-        <v>17000.0</v>
-      </c>
-      <c r="L46" s="7">
-        <v>19000.0</v>
-      </c>
-    </row>
-    <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="7">
-        <v>37000.0</v>
-      </c>
-    </row>
-    <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="7">
-        <v>8000.0</v>
-      </c>
-      <c r="K48" s="7">
-        <v>10000.0</v>
-      </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="8"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
+      <c r="A49" s="2"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="8"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
+      <c r="A50" s="2"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="8"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
+      <c r="A51" s="2"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="8"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
+      <c r="A52" s="2"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="8"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
+      <c r="A53" s="2"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="8"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
+      <c r="A54" s="2"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="8"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
+      <c r="A55" s="2"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="8"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="6"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
+      <c r="A56" s="2"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
     </row>
     <row r="57" ht="15.75" customHeight="1"/>
     <row r="58" ht="15.75" customHeight="1"/>
@@ -2512,93 +2336,72 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="17.63"/>
-    <col customWidth="1" min="3" max="27" width="9.38"/>
+    <col customWidth="1" min="1" max="1" width="17.63"/>
+    <col customWidth="1" min="2" max="26" width="9.38"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="10" t="s">
+      <c r="B1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="10" t="s">
+    </row>
+    <row r="2" ht="12.75" customHeight="1">
+      <c r="A2" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E2" s="5">
+        <v>110000.0</v>
+      </c>
+    </row>
+    <row r="3" ht="12.75" customHeight="1">
+      <c r="A3" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="E3" s="5">
+        <v>97000.0</v>
+      </c>
+    </row>
+    <row r="4" ht="12.75" customHeight="1">
+      <c r="A4" s="6" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="9" t="s">
+      <c r="B4" s="5">
+        <v>46000.0</v>
+      </c>
+    </row>
+    <row r="5" ht="12.75" customHeight="1">
+      <c r="A5" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B5" s="5">
+        <v>67000.0</v>
+      </c>
+    </row>
+    <row r="6" ht="12.75" customHeight="1">
+      <c r="A6" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F2" s="7">
-        <v>110000.0</v>
-      </c>
-    </row>
-    <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" s="10" t="s">
+      <c r="B6" s="5">
+        <v>83000.0</v>
+      </c>
+    </row>
+    <row r="7" ht="12.75" customHeight="1">
+      <c r="A7" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="7">
-        <v>97000.0</v>
-      </c>
-    </row>
-    <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" s="7">
-        <v>46000.0</v>
-      </c>
-    </row>
-    <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="7">
-        <v>67000.0</v>
-      </c>
-    </row>
-    <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" s="7">
-        <v>83000.0</v>
-      </c>
-    </row>
-    <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C7" s="7">
+      <c r="B7" s="5">
         <v>39000.0</v>
       </c>
     </row>

</xml_diff>